<commit_message>
añadí la columna de inicial y agregué las variables de decisión
</commit_message>
<xml_diff>
--- a/conf_file.xlsx
+++ b/conf_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mini_proyecto_de_optimizacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{392C8F40-F179-4603-BDA4-3C0918CBD0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA254E98-C949-487A-A6C6-8FA48A58C3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{F52739E3-C600-44DC-84B9-5DC827D8A67D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F52739E3-C600-44DC-84B9-5DC827D8A67D}"/>
   </bookViews>
   <sheets>
     <sheet name="Arcs" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arcs!$A$1:$E$11</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Node_end!$A$1:$D$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Node_start!$A$1:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Node_start!$A$1:$E$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Nodes!$A$1:$D$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
   <si>
     <t>Node_start</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Cost_node</t>
+  </si>
+  <si>
+    <t>Initial</t>
   </si>
 </sst>
 </file>
@@ -101,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -176,12 +179,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -193,34 +196,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -249,14 +253,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{723A5978-696A-4CAE-862A-3234B911E106}" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{723A5978-696A-4CAE-862A-3234B911E106}" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E11" xr:uid="{9B779D43-810E-457B-8649-B525413CC079}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{89DBCA3F-648A-4C3C-B75F-C81CBDCD2A59}" name="Node_start" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{3382B0E1-FD71-48E2-9B24-342E60D91B54}" name="Node_end" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{D397FD23-0663-464D-9B40-A6153D97989B}" name="Min_flow" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{09F128A5-B8F9-43D8-889B-C7EDE6B53558}" name="Max_flow" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{5B1BAD43-82E0-4480-AF1A-293AB7A12804}" name="Cost_arc" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{89DBCA3F-648A-4C3C-B75F-C81CBDCD2A59}" name="Node_start" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{3382B0E1-FD71-48E2-9B24-342E60D91B54}" name="Node_end" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{D397FD23-0663-464D-9B40-A6153D97989B}" name="Min_flow" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{09F128A5-B8F9-43D8-889B-C7EDE6B53558}" name="Max_flow" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{5B1BAD43-82E0-4480-AF1A-293AB7A12804}" name="Cost_arc" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -561,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B779D43-810E-457B-8649-B525413CC079}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,7 +575,7 @@
     <col min="2" max="2" width="11.453125" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.7265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.08984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="2" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -588,24 +592,24 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
         <v>12</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="10">
         <v>1.1000000000000001</v>
       </c>
     </row>
@@ -627,19 +631,19 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
         <v>33</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="10">
         <v>6.7</v>
       </c>
     </row>
@@ -661,19 +665,19 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
         <v>24</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="10">
         <v>9.6</v>
       </c>
     </row>
@@ -695,19 +699,19 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
         <v>13</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="10">
         <v>5.0999999999999996</v>
       </c>
     </row>
@@ -729,19 +733,19 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
         <v>30</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="10">
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -773,18 +777,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61774104-72A8-4F69-90E7-77193C58F2AC}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -794,26 +798,32 @@
       <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
         <v>2000</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="10">
         <v>3.65</v>
       </c>
+      <c r="E2" s="3">
+        <v>1000</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D2" xr:uid="{61774104-72A8-4F69-90E7-77193C58F2AC}"/>
+  <autoFilter ref="A1:E2" xr:uid="{61774104-72A8-4F69-90E7-77193C58F2AC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -824,10 +834,13 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="8.7265625" style="11"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
@@ -839,7 +852,7 @@
       <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -847,13 +860,13 @@
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
         <v>1999</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="10">
         <v>4.6500000000000004</v>
       </c>
     </row>
@@ -868,15 +881,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C308F50B-FAAB-46EB-A03C-44C61742B1A1}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -889,7 +902,7 @@
       <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>16</v>
       </c>
     </row>
@@ -897,27 +910,27 @@
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6">
-        <v>0</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
         <v>1500</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="10">
         <v>1.65</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9">
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
         <v>1400</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <v>5.65</v>
       </c>
     </row>
@@ -925,27 +938,27 @@
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
         <v>3000</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="10">
         <v>7.65</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9">
-        <v>0</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
         <v>1000</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>9.65</v>
       </c>
     </row>
@@ -953,27 +966,27 @@
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
         <v>1000</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="10">
         <v>1.65</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="9">
-        <v>0</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
         <v>3000</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="8">
         <v>5.98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificación en el archivo de configuración
</commit_message>
<xml_diff>
--- a/conf_file.xlsx
+++ b/conf_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mini_proyecto_de_optimizacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA254E98-C949-487A-A6C6-8FA48A58C3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546B1D4F-7287-49FD-A1AD-F855D1B1CAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F52739E3-C600-44DC-84B9-5DC827D8A67D}"/>
   </bookViews>
@@ -20,9 +20,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arcs!$A$1:$E$11</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Node_end!$A$1:$D$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Node_start!$A$1:$E$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Nodes!$A$1:$D$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Node_end!$A$1:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Node_start!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Nodes!$A$1:$E$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
   <si>
     <t>Node_start</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Initial</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -143,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -175,11 +181,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -212,11 +246,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -253,14 +296,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{723A5978-696A-4CAE-862A-3234B911E106}" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E11" xr:uid="{9B779D43-810E-457B-8649-B525413CC079}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{89DBCA3F-648A-4C3C-B75F-C81CBDCD2A59}" name="Node_start" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{3382B0E1-FD71-48E2-9B24-342E60D91B54}" name="Node_end" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{D397FD23-0663-464D-9B40-A6153D97989B}" name="Min_flow" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{09F128A5-B8F9-43D8-889B-C7EDE6B53558}" name="Max_flow" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{5B1BAD43-82E0-4480-AF1A-293AB7A12804}" name="Cost_arc" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{723A5978-696A-4CAE-862A-3234B911E106}" name="Table1" displayName="Table1" ref="A1:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F11" xr:uid="{9B779D43-810E-457B-8649-B525413CC079}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{89DBCA3F-648A-4C3C-B75F-C81CBDCD2A59}" name="Node_start" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{3382B0E1-FD71-48E2-9B24-342E60D91B54}" name="Node_end" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{D397FD23-0663-464D-9B40-A6153D97989B}" name="Min_flow" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{09F128A5-B8F9-43D8-889B-C7EDE6B53558}" name="Max_flow" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{5B1BAD43-82E0-4480-AF1A-293AB7A12804}" name="Cost_arc" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{5BBBD529-CA19-48E3-A00B-E1CE97998502}" name="Active" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -563,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B779D43-810E-457B-8649-B525413CC079}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,7 +623,7 @@
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,8 +639,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -612,8 +659,11 @@
       <c r="E2" s="10">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -629,8 +679,11 @@
       <c r="E3" s="2">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -646,8 +699,11 @@
       <c r="E4" s="10">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -663,8 +719,11 @@
       <c r="E5" s="2">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -680,8 +739,11 @@
       <c r="E6" s="10">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -697,8 +759,11 @@
       <c r="E7" s="2">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -714,8 +779,11 @@
       <c r="E8" s="10">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -731,8 +799,11 @@
       <c r="E9" s="2">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -748,8 +819,11 @@
       <c r="E10" s="10">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -764,6 +838,9 @@
       </c>
       <c r="E11" s="2">
         <v>10.5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -777,10 +854,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61774104-72A8-4F69-90E7-77193C58F2AC}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -788,7 +865,7 @@
     <col min="4" max="4" width="9.7265625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -804,8 +881,11 @@
       <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -821,9 +901,12 @@
       <c r="E2" s="3">
         <v>1000</v>
       </c>
+      <c r="F2" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E2" xr:uid="{61774104-72A8-4F69-90E7-77193C58F2AC}"/>
+  <autoFilter ref="A1:F2" xr:uid="{61774104-72A8-4F69-90E7-77193C58F2AC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -831,10 +914,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EBE9CA9-8A94-42D7-BA5E-CDB77882ACCF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -842,7 +925,7 @@
     <col min="4" max="4" width="8.7265625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -855,8 +938,11 @@
       <c r="D1" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -869,9 +955,12 @@
       <c r="D2" s="10">
         <v>4.6500000000000004</v>
       </c>
+      <c r="E2" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D2" xr:uid="{7EBE9CA9-8A94-42D7-BA5E-CDB77882ACCF}"/>
+  <autoFilter ref="A1:E2" xr:uid="{7EBE9CA9-8A94-42D7-BA5E-CDB77882ACCF}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -879,10 +968,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C308F50B-FAAB-46EB-A03C-44C61742B1A1}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -892,7 +981,7 @@
     <col min="4" max="4" width="9.81640625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
@@ -905,8 +994,11 @@
       <c r="D1" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -917,10 +1009,13 @@
         <v>1500</v>
       </c>
       <c r="D2" s="10">
-        <v>1.65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1.75</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -933,8 +1028,11 @@
       <c r="D3" s="8">
         <v>5.65</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -947,8 +1045,11 @@
       <c r="D4" s="10">
         <v>7.65</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -961,8 +1062,11 @@
       <c r="D5" s="8">
         <v>9.65</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -975,8 +1079,11 @@
       <c r="D6" s="10">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
@@ -989,9 +1096,12 @@
       <c r="D7" s="8">
         <v>5.98</v>
       </c>
+      <c r="E7" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D7" xr:uid="{C308F50B-FAAB-46EB-A03C-44C61742B1A1}"/>
+  <autoFilter ref="A1:E7" xr:uid="{C308F50B-FAAB-46EB-A03C-44C61742B1A1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambios en el archivo de configuración + agregación de la función objetivo y los parametros
</commit_message>
<xml_diff>
--- a/conf_file.xlsx
+++ b/conf_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mini_proyecto_de_optimizacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546B1D4F-7287-49FD-A1AD-F855D1B1CAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B9F92F-E8F7-4BC3-AD73-6DC71660462A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F52739E3-C600-44DC-84B9-5DC827D8A67D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{F52739E3-C600-44DC-84B9-5DC827D8A67D}"/>
   </bookViews>
   <sheets>
     <sheet name="Arcs" sheetId="1" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B779D43-810E-457B-8649-B525413CC079}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -857,7 +857,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -917,7 +917,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -970,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C308F50B-FAAB-46EB-A03C-44C61742B1A1}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1043,7 +1043,7 @@
         <v>3000</v>
       </c>
       <c r="D4" s="10">
-        <v>7.65</v>
+        <v>7.34</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Cambio en el costo
</commit_message>
<xml_diff>
--- a/conf_file.xlsx
+++ b/conf_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mini_proyecto_de_optimizacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B9F92F-E8F7-4BC3-AD73-6DC71660462A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89997D7E-1F91-4B62-B92B-A2C9E2979825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{F52739E3-C600-44DC-84B9-5DC827D8A67D}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" activeTab="3" xr2:uid="{F52739E3-C600-44DC-84B9-5DC827D8A67D}"/>
   </bookViews>
   <sheets>
     <sheet name="Arcs" sheetId="1" r:id="rId1"/>
@@ -971,7 +971,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1026,7 +1026,7 @@
         <v>1400</v>
       </c>
       <c r="D3" s="8">
-        <v>5.65</v>
+        <v>0.65</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>19</v>
@@ -1043,7 +1043,7 @@
         <v>3000</v>
       </c>
       <c r="D4" s="10">
-        <v>7.34</v>
+        <v>0.34</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>19</v>
@@ -1060,7 +1060,7 @@
         <v>1000</v>
       </c>
       <c r="D5" s="8">
-        <v>9.65</v>
+        <v>0.65</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>19</v>

</xml_diff>